<commit_message>
Pagarināta laika līnija Excel dok. - "Darbs plāns"
</commit_message>
<xml_diff>
--- a/Dok/2. Proj2_work_plan.xlsx
+++ b/Dok/2. Proj2_work_plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KRISTS\DOKUMENTI\STUDIJAS (MAĢISTRS)\Kursi\2. kurss 1. semestris\Kvalifikācijas prakse II\Proj2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krists\Documents\GitHub\Arnim\Dok\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -602,7 +602,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1887,14 +1887,14 @@
       <c r="T23" s="16"/>
       <c r="U23" s="16"/>
       <c r="V23" s="16"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="15"/>
-      <c r="Y23" s="15"/>
-      <c r="Z23" s="15"/>
-      <c r="AA23" s="15"/>
-      <c r="AB23" s="15"/>
-      <c r="AC23" s="15"/>
-      <c r="AD23" s="15"/>
+      <c r="W23" s="16"/>
+      <c r="X23" s="16"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="16"/>
+      <c r="AB23" s="16"/>
+      <c r="AC23" s="16"/>
+      <c r="AD23" s="16"/>
       <c r="AE23" s="15"/>
       <c r="AF23" s="15"/>
       <c r="AG23" s="15"/>

</xml_diff>